<commit_message>
added sheets to catalog, did alittle formatting, region list in a decent spot, race list pretty much done, working on race by region list.
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jquigley\Desktop\git\npc+catalouger\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jquigley\Desktop\git\npc_catalog\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -13,6 +13,9 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Races" sheetId="4" r:id="rId3"/>
+    <sheet name="Races by Region" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -24,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="12">
   <si>
     <t>Race</t>
   </si>
@@ -42,6 +45,24 @@
   </si>
   <si>
     <t>Title</t>
+  </si>
+  <si>
+    <t>Continent</t>
+  </si>
+  <si>
+    <t>Races</t>
+  </si>
+  <si>
+    <t>Region #</t>
+  </si>
+  <si>
+    <t>Northern Austaria</t>
+  </si>
+  <si>
+    <t>Dayanese</t>
+  </si>
+  <si>
+    <t>Races by Region</t>
   </si>
 </sst>
 </file>
@@ -65,7 +86,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="19">
     <border>
       <left/>
       <right/>
@@ -73,12 +94,282 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -359,35 +650,385 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.33203125" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>5</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="17.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
+      <c r="J1" s="3"/>
+      <c r="K1" s="4"/>
+    </row>
+    <row r="2" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="2"/>
+      <c r="B2" s="7">
+        <v>1</v>
+      </c>
+      <c r="C2" s="5">
+        <v>2</v>
+      </c>
+      <c r="D2" s="5">
+        <v>3</v>
+      </c>
+      <c r="E2" s="5">
+        <v>4</v>
+      </c>
+      <c r="F2" s="5">
+        <v>5</v>
+      </c>
+      <c r="G2" s="5">
+        <v>6</v>
+      </c>
+      <c r="H2" s="5">
+        <v>7</v>
+      </c>
+      <c r="I2" s="5">
+        <v>8</v>
+      </c>
+      <c r="J2" s="5">
+        <v>9</v>
+      </c>
+      <c r="K2" s="6">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:K1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H17"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="20.44140625" style="22" customWidth="1"/>
+    <col min="2" max="16384" width="13.21875" hidden="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="20" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2" s="21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3" s="22">
+        <v>2</v>
+      </c>
+      <c r="C3" s="18"/>
+      <c r="D3" s="19"/>
+      <c r="E3" s="19"/>
+      <c r="F3" s="19"/>
+      <c r="G3" s="19"/>
+      <c r="H3" s="18"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A4" s="22">
+        <v>4</v>
+      </c>
+      <c r="C4" s="18"/>
+      <c r="D4" s="19"/>
+      <c r="E4" s="19"/>
+      <c r="F4" s="19"/>
+      <c r="G4" s="19"/>
+      <c r="H4" s="18"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5" s="22">
+        <v>5</v>
+      </c>
+      <c r="C5" s="18"/>
+      <c r="D5" s="19"/>
+      <c r="E5" s="19"/>
+      <c r="F5" s="19"/>
+      <c r="G5" s="19"/>
+      <c r="H5" s="18"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A6" s="22">
+        <v>6</v>
+      </c>
+      <c r="C6" s="18"/>
+      <c r="D6" s="19"/>
+      <c r="E6" s="19"/>
+      <c r="F6" s="19"/>
+      <c r="G6" s="19"/>
+      <c r="H6" s="18"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A7" s="22">
+        <v>7</v>
+      </c>
+      <c r="C7" s="18"/>
+      <c r="D7" s="19"/>
+      <c r="E7" s="19"/>
+      <c r="F7" s="19"/>
+      <c r="G7" s="19"/>
+      <c r="H7" s="18"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A8" s="22">
+        <v>8</v>
+      </c>
+      <c r="C8" s="18"/>
+      <c r="D8" s="19"/>
+      <c r="E8" s="19"/>
+      <c r="F8" s="19"/>
+      <c r="G8" s="19"/>
+      <c r="H8" s="18"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="C9" s="18"/>
+      <c r="D9" s="19"/>
+      <c r="E9" s="19"/>
+      <c r="F9" s="19"/>
+      <c r="G9" s="19"/>
+      <c r="H9" s="18"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="C10" s="18"/>
+      <c r="D10" s="19"/>
+      <c r="E10" s="19"/>
+      <c r="F10" s="19"/>
+      <c r="G10" s="19"/>
+      <c r="H10" s="18"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="C11" s="18"/>
+      <c r="D11" s="18"/>
+      <c r="E11" s="18"/>
+      <c r="F11" s="18"/>
+      <c r="G11" s="18"/>
+      <c r="H11" s="18"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="C12" s="18"/>
+      <c r="D12" s="18"/>
+      <c r="E12" s="18"/>
+      <c r="F12" s="18"/>
+      <c r="G12" s="18"/>
+      <c r="H12" s="18"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="C13" s="18"/>
+      <c r="D13" s="18"/>
+      <c r="E13" s="18"/>
+      <c r="F13" s="18"/>
+      <c r="G13" s="18"/>
+      <c r="H13" s="18"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="C14" s="18"/>
+      <c r="D14" s="18"/>
+      <c r="E14" s="18"/>
+      <c r="F14" s="18"/>
+      <c r="G14" s="18"/>
+      <c r="H14" s="18"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="C15" s="18"/>
+      <c r="D15" s="18"/>
+      <c r="E15" s="18"/>
+      <c r="F15" s="18"/>
+      <c r="G15" s="18"/>
+      <c r="H15" s="18"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="C16" s="18"/>
+      <c r="D16" s="18"/>
+      <c r="E16" s="18"/>
+      <c r="F16" s="18"/>
+      <c r="G16" s="18"/>
+      <c r="H16" s="18"/>
+    </row>
+    <row r="17" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C17" s="18"/>
+      <c r="D17" s="18"/>
+      <c r="E17" s="18"/>
+      <c r="F17" s="18"/>
+      <c r="G17" s="18"/>
+      <c r="H17" s="18"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="17.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="14" t="str">
+        <f>IF(Sheet2!A3 = 0, "",Sheet2!A3)</f>
+        <v>Northern Austaria</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="17">
+        <f>IF(Sheet2!B2 = 0, "",Sheet2!B2)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5" s="16" t="str">
+        <f>IF(Sheet2!B3 = 0, "",Sheet2!B3)</f>
+        <v>Dayanese</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="8"/>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" s="11"/>
+      <c r="B7" s="8"/>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" s="11"/>
+      <c r="B8" s="8"/>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" s="11"/>
+      <c r="B9" s="8"/>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" s="11"/>
+      <c r="B10" s="8"/>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" s="11"/>
+      <c r="B11" s="8"/>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12" s="11"/>
+      <c r="B12" s="8"/>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13" s="11"/>
+      <c r="B13" s="8"/>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14" s="11"/>
+      <c r="B14" s="8"/>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15" s="11"/>
+      <c r="B15" s="8"/>
+    </row>
+    <row r="16" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="12"/>
+      <c r="B16" s="9"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A6:A16"/>
+  </mergeCells>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B6:B16">
+      <formula1>"Races$A1:$A4"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>